<commit_message>
Creada la estructura de la base de datos
- Con este blueprint de las tablas ya se puede trabajar en la aplicacion
</commit_message>
<xml_diff>
--- a/analisis de metas.xlsx
+++ b/analisis de metas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="12">
   <si>
     <t>Outs</t>
   </si>
@@ -28,6 +28,9 @@
   </si>
   <si>
     <t>Area</t>
+  </si>
+  <si>
+    <t>Meta</t>
   </si>
   <si>
     <t>OSAS</t>
@@ -55,9 +58,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="28"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -84,9 +94,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,27 +392,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:I35"/>
+  <dimension ref="A2:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9">
-      <c r="B3" t="s">
+    <row r="2" spans="1:9">
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="36">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -413,19 +438,19 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" t="s">
         <v>10</v>
       </c>
-      <c r="F4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" t="s">
-        <v>9</v>
-      </c>
       <c r="H4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -433,32 +458,33 @@
         <v>2015</v>
       </c>
       <c r="B5">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E5" s="1">
         <f>DATE(A5,B5,C5)</f>
-        <v>42339</v>
+        <v>42309</v>
       </c>
       <c r="F5">
-        <v>53</v>
+        <f>$F$2*C5</f>
+        <v>40</v>
       </c>
       <c r="G5">
         <f>WEEKDAY(DATE(A5,B5,C5))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H5">
         <f>$F$5*G5</f>
-        <v>159</v>
+        <v>40</v>
       </c>
       <c r="I5">
         <f>$F$5*31</f>
-        <v>1643</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -467,32 +493,33 @@
       </c>
       <c r="B6">
         <f>$B$5</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" ref="E6:E35" si="0">DATE(A6,B6,C6)</f>
-        <v>42340</v>
+        <v>42310</v>
       </c>
       <c r="F6">
-        <v>106</v>
+        <f t="shared" ref="F6:F35" si="1">$F$2*C6</f>
+        <v>80</v>
       </c>
       <c r="G6">
         <f>WEEKDAY(DATE(A6,B6,C6))</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H6">
         <f>$F$5*G6</f>
-        <v>212</v>
+        <v>80</v>
       </c>
       <c r="I6">
         <f>$F$5*31</f>
-        <v>1643</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -500,33 +527,34 @@
         <v>2015</v>
       </c>
       <c r="B7">
-        <f t="shared" ref="B7:B35" si="1">$B$5</f>
-        <v>12</v>
+        <f t="shared" ref="B7:B35" si="2">$B$5</f>
+        <v>11</v>
       </c>
       <c r="C7">
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>42341</v>
+        <v>42311</v>
       </c>
       <c r="F7">
-        <v>159</v>
+        <f t="shared" si="1"/>
+        <v>120</v>
       </c>
       <c r="G7">
         <f>WEEKDAY(DATE(A7,B7,C7))</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H7">
         <f>$F$5*G7</f>
-        <v>265</v>
+        <v>120</v>
       </c>
       <c r="I7">
         <f>$F$5*31</f>
-        <v>1643</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -534,33 +562,34 @@
         <v>2015</v>
       </c>
       <c r="B8">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="C8">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>42342</v>
+        <v>42312</v>
       </c>
       <c r="F8">
-        <v>212</v>
+        <f t="shared" si="1"/>
+        <v>160</v>
       </c>
       <c r="G8">
         <f>WEEKDAY(DATE(A8,B8,C8))</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H8">
         <f>$F$5*G8</f>
-        <v>318</v>
+        <v>160</v>
       </c>
       <c r="I8">
         <f>$F$5*31</f>
-        <v>1643</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -568,33 +597,34 @@
         <v>2015</v>
       </c>
       <c r="B9">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="C9">
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>42343</v>
+        <v>42313</v>
       </c>
       <c r="F9">
-        <v>265</v>
+        <f t="shared" si="1"/>
+        <v>200</v>
       </c>
       <c r="G9">
         <f>WEEKDAY(DATE(A9,B9,C9))</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H9">
         <f>$F$5*G9</f>
-        <v>371</v>
+        <v>200</v>
       </c>
       <c r="I9">
         <f>$F$5*31</f>
-        <v>1643</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -602,33 +632,34 @@
         <v>2015</v>
       </c>
       <c r="B10">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="C10">
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>42344</v>
+        <v>42314</v>
       </c>
       <c r="F10">
-        <v>318</v>
+        <f t="shared" si="1"/>
+        <v>240</v>
       </c>
       <c r="G10">
         <f>WEEKDAY(DATE(A10,B10,C10))</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H10">
         <f>$F$5*G10</f>
-        <v>53</v>
+        <v>240</v>
       </c>
       <c r="I10">
         <f>$F$5*31</f>
-        <v>1643</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -636,33 +667,34 @@
         <v>2015</v>
       </c>
       <c r="B11">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="C11">
         <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>42345</v>
+        <v>42315</v>
       </c>
       <c r="F11">
-        <v>371</v>
+        <f t="shared" si="1"/>
+        <v>280</v>
       </c>
       <c r="G11">
         <f>WEEKDAY(DATE(A11,B11,C11))</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H11">
         <f>$F$5*G11</f>
-        <v>106</v>
+        <v>280</v>
       </c>
       <c r="I11">
         <f>$F$5*31</f>
-        <v>1643</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -670,33 +702,34 @@
         <v>2015</v>
       </c>
       <c r="B12">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="C12">
         <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>42346</v>
+        <v>42316</v>
       </c>
       <c r="F12">
-        <v>424</v>
+        <f t="shared" si="1"/>
+        <v>320</v>
       </c>
       <c r="G12">
         <f>WEEKDAY(DATE(A12,B12,C12))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H12">
         <f>$F$5*G12</f>
-        <v>159</v>
+        <v>40</v>
       </c>
       <c r="I12">
         <f>$F$5*31</f>
-        <v>1643</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -704,33 +737,34 @@
         <v>2015</v>
       </c>
       <c r="B13">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="C13">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>42347</v>
+        <v>42317</v>
       </c>
       <c r="F13">
-        <v>477</v>
+        <f t="shared" si="1"/>
+        <v>360</v>
       </c>
       <c r="G13">
         <f>WEEKDAY(DATE(A13,B13,C13))</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H13">
         <f>$F$5*G13</f>
-        <v>212</v>
+        <v>80</v>
       </c>
       <c r="I13">
         <f>$F$5*31</f>
-        <v>1643</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -738,33 +772,34 @@
         <v>2015</v>
       </c>
       <c r="B14">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="C14">
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>42348</v>
+        <v>42318</v>
       </c>
       <c r="F14">
-        <v>530</v>
+        <f t="shared" si="1"/>
+        <v>400</v>
       </c>
       <c r="G14">
         <f>WEEKDAY(DATE(A14,B14,C14))</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H14">
         <f>$F$5*G14</f>
-        <v>265</v>
+        <v>120</v>
       </c>
       <c r="I14">
         <f>$F$5*31</f>
-        <v>1643</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -772,33 +807,34 @@
         <v>2015</v>
       </c>
       <c r="B15">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="C15">
         <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>42349</v>
+        <v>42319</v>
       </c>
       <c r="F15">
-        <v>583</v>
+        <f t="shared" si="1"/>
+        <v>440</v>
       </c>
       <c r="G15">
         <f>WEEKDAY(DATE(A15,B15,C15))</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H15">
         <f>$F$5*G15</f>
-        <v>318</v>
+        <v>160</v>
       </c>
       <c r="I15">
         <f>$F$5*31</f>
-        <v>1643</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -806,33 +842,34 @@
         <v>2015</v>
       </c>
       <c r="B16">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="C16">
         <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>42350</v>
+        <v>42320</v>
       </c>
       <c r="F16">
-        <v>636</v>
+        <f t="shared" si="1"/>
+        <v>480</v>
       </c>
       <c r="G16">
         <f>WEEKDAY(DATE(A16,B16,C16))</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H16">
         <f>$F$5*G16</f>
-        <v>371</v>
+        <v>200</v>
       </c>
       <c r="I16">
         <f>$F$5*31</f>
-        <v>1643</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -840,33 +877,34 @@
         <v>2015</v>
       </c>
       <c r="B17">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="C17">
         <v>13</v>
       </c>
       <c r="D17" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>42351</v>
+        <v>42321</v>
       </c>
       <c r="F17">
-        <v>689</v>
+        <f t="shared" si="1"/>
+        <v>520</v>
       </c>
       <c r="G17">
         <f>WEEKDAY(DATE(A17,B17,C17))</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H17">
         <f>$F$5*G17</f>
-        <v>53</v>
+        <v>240</v>
       </c>
       <c r="I17">
         <f>$F$5*31</f>
-        <v>1643</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -874,33 +912,34 @@
         <v>2015</v>
       </c>
       <c r="B18">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="C18">
         <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>42352</v>
+        <v>42322</v>
       </c>
       <c r="F18">
-        <v>742</v>
+        <f t="shared" si="1"/>
+        <v>560</v>
       </c>
       <c r="G18">
         <f>WEEKDAY(DATE(A18,B18,C18))</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H18">
         <f>$F$5*G18</f>
-        <v>106</v>
+        <v>280</v>
       </c>
       <c r="I18">
         <f>$F$5*31</f>
-        <v>1643</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -908,33 +947,34 @@
         <v>2015</v>
       </c>
       <c r="B19">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="C19">
         <v>15</v>
       </c>
       <c r="D19" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>42353</v>
+        <v>42323</v>
       </c>
       <c r="F19">
-        <v>795</v>
+        <f t="shared" si="1"/>
+        <v>600</v>
       </c>
       <c r="G19">
         <f>WEEKDAY(DATE(A19,B19,C19))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H19">
         <f>$F$5*G19</f>
-        <v>159</v>
+        <v>40</v>
       </c>
       <c r="I19">
         <f>$F$5*31</f>
-        <v>1643</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -942,33 +982,34 @@
         <v>2015</v>
       </c>
       <c r="B20">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="C20">
         <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>42354</v>
+        <v>42324</v>
       </c>
       <c r="F20">
-        <v>848</v>
+        <f t="shared" si="1"/>
+        <v>640</v>
       </c>
       <c r="G20">
         <f>WEEKDAY(DATE(A20,B20,C20))</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H20">
         <f>$F$5*G20</f>
-        <v>212</v>
+        <v>80</v>
       </c>
       <c r="I20">
         <f>$F$5*31</f>
-        <v>1643</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -976,33 +1017,34 @@
         <v>2015</v>
       </c>
       <c r="B21">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="C21">
         <v>17</v>
       </c>
       <c r="D21" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>42355</v>
+        <v>42325</v>
       </c>
       <c r="F21">
-        <v>901</v>
+        <f t="shared" si="1"/>
+        <v>680</v>
       </c>
       <c r="G21">
         <f>WEEKDAY(DATE(A21,B21,C21))</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H21">
         <f>$F$5*G21</f>
-        <v>265</v>
+        <v>120</v>
       </c>
       <c r="I21">
         <f>$F$5*31</f>
-        <v>1643</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1010,33 +1052,34 @@
         <v>2015</v>
       </c>
       <c r="B22">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="C22">
         <v>18</v>
       </c>
       <c r="D22" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>42356</v>
+        <v>42326</v>
       </c>
       <c r="F22">
-        <v>954</v>
+        <f t="shared" si="1"/>
+        <v>720</v>
       </c>
       <c r="G22">
         <f>WEEKDAY(DATE(A22,B22,C22))</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H22">
         <f>$F$5*G22</f>
-        <v>318</v>
+        <v>160</v>
       </c>
       <c r="I22">
         <f>$F$5*31</f>
-        <v>1643</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1044,33 +1087,34 @@
         <v>2015</v>
       </c>
       <c r="B23">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="C23">
         <v>19</v>
       </c>
       <c r="D23" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>42357</v>
+        <v>42327</v>
       </c>
       <c r="F23">
-        <v>1007</v>
+        <f t="shared" si="1"/>
+        <v>760</v>
       </c>
       <c r="G23">
         <f>WEEKDAY(DATE(A23,B23,C23))</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H23">
         <f>$F$5*G23</f>
-        <v>371</v>
+        <v>200</v>
       </c>
       <c r="I23">
         <f>$F$5*31</f>
-        <v>1643</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1078,33 +1122,34 @@
         <v>2015</v>
       </c>
       <c r="B24">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="C24">
         <v>20</v>
       </c>
       <c r="D24" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>42358</v>
+        <v>42328</v>
       </c>
       <c r="F24">
-        <v>1060</v>
+        <f t="shared" si="1"/>
+        <v>800</v>
       </c>
       <c r="G24">
         <f>WEEKDAY(DATE(A24,B24,C24))</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H24">
         <f>$F$5*G24</f>
-        <v>53</v>
+        <v>240</v>
       </c>
       <c r="I24">
         <f>$F$5*31</f>
-        <v>1643</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1112,33 +1157,34 @@
         <v>2015</v>
       </c>
       <c r="B25">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="C25">
         <v>21</v>
       </c>
       <c r="D25" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>42359</v>
+        <v>42329</v>
       </c>
       <c r="F25">
-        <v>1113</v>
+        <f t="shared" si="1"/>
+        <v>840</v>
       </c>
       <c r="G25">
         <f>WEEKDAY(DATE(A25,B25,C25))</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H25">
         <f>$F$5*G25</f>
-        <v>106</v>
+        <v>280</v>
       </c>
       <c r="I25">
         <f>$F$5*31</f>
-        <v>1643</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1146,33 +1192,34 @@
         <v>2015</v>
       </c>
       <c r="B26">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="C26">
         <v>22</v>
       </c>
       <c r="D26" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>42360</v>
+        <v>42330</v>
       </c>
       <c r="F26">
-        <v>1166</v>
+        <f t="shared" si="1"/>
+        <v>880</v>
       </c>
       <c r="G26">
         <f>WEEKDAY(DATE(A26,B26,C26))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H26">
         <f>$F$5*G26</f>
-        <v>159</v>
+        <v>40</v>
       </c>
       <c r="I26">
         <f>$F$5*31</f>
-        <v>1643</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1180,33 +1227,34 @@
         <v>2015</v>
       </c>
       <c r="B27">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="C27">
         <v>23</v>
       </c>
       <c r="D27" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>42361</v>
+        <v>42331</v>
       </c>
       <c r="F27">
-        <v>1219</v>
+        <f t="shared" si="1"/>
+        <v>920</v>
       </c>
       <c r="G27">
         <f>WEEKDAY(DATE(A27,B27,C27))</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H27">
         <f>$F$5*G27</f>
-        <v>212</v>
+        <v>80</v>
       </c>
       <c r="I27">
         <f>$F$5*31</f>
-        <v>1643</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1214,33 +1262,34 @@
         <v>2015</v>
       </c>
       <c r="B28">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="C28">
         <v>24</v>
       </c>
       <c r="D28" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>42362</v>
+        <v>42332</v>
       </c>
       <c r="F28">
-        <v>1272</v>
+        <f t="shared" si="1"/>
+        <v>960</v>
       </c>
       <c r="G28">
         <f>WEEKDAY(DATE(A28,B28,C28))</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H28">
         <f>$F$5*G28</f>
-        <v>265</v>
+        <v>120</v>
       </c>
       <c r="I28">
         <f>$F$5*31</f>
-        <v>1643</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1248,33 +1297,34 @@
         <v>2015</v>
       </c>
       <c r="B29">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="C29">
         <v>25</v>
       </c>
       <c r="D29" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>42363</v>
+        <v>42333</v>
       </c>
       <c r="F29">
-        <v>1325</v>
+        <f t="shared" si="1"/>
+        <v>1000</v>
       </c>
       <c r="G29">
         <f>WEEKDAY(DATE(A29,B29,C29))</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H29">
         <f>$F$5*G29</f>
-        <v>318</v>
+        <v>160</v>
       </c>
       <c r="I29">
         <f>$F$5*31</f>
-        <v>1643</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1282,33 +1332,34 @@
         <v>2015</v>
       </c>
       <c r="B30">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="C30">
         <v>26</v>
       </c>
       <c r="D30" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>42364</v>
+        <v>42334</v>
       </c>
       <c r="F30">
-        <v>1378</v>
+        <f t="shared" si="1"/>
+        <v>1040</v>
       </c>
       <c r="G30">
         <f>WEEKDAY(DATE(A30,B30,C30))</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H30">
         <f>$F$5*G30</f>
-        <v>371</v>
+        <v>200</v>
       </c>
       <c r="I30">
         <f>$F$5*31</f>
-        <v>1643</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1316,33 +1367,34 @@
         <v>2015</v>
       </c>
       <c r="B31">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="C31">
         <v>27</v>
       </c>
       <c r="D31" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>42365</v>
+        <v>42335</v>
       </c>
       <c r="F31">
-        <v>1431</v>
+        <f t="shared" si="1"/>
+        <v>1080</v>
       </c>
       <c r="G31">
         <f>WEEKDAY(DATE(A31,B31,C31))</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H31">
         <f>$F$5*G31</f>
-        <v>53</v>
+        <v>240</v>
       </c>
       <c r="I31">
         <f>$F$5*31</f>
-        <v>1643</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1350,33 +1402,34 @@
         <v>2015</v>
       </c>
       <c r="B32">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="C32">
         <v>28</v>
       </c>
       <c r="D32" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>42366</v>
+        <v>42336</v>
       </c>
       <c r="F32">
-        <v>1484</v>
+        <f t="shared" si="1"/>
+        <v>1120</v>
       </c>
       <c r="G32">
         <f>WEEKDAY(DATE(A32,B32,C32))</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H32">
         <f>$F$5*G32</f>
-        <v>106</v>
+        <v>280</v>
       </c>
       <c r="I32">
         <f>$F$5*31</f>
-        <v>1643</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1384,33 +1437,34 @@
         <v>2015</v>
       </c>
       <c r="B33">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="C33">
         <v>29</v>
       </c>
       <c r="D33" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>42367</v>
+        <v>42337</v>
       </c>
       <c r="F33">
-        <v>1537</v>
+        <f t="shared" si="1"/>
+        <v>1160</v>
       </c>
       <c r="G33">
         <f>WEEKDAY(DATE(A33,B33,C33))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H33">
         <f>$F$5*G33</f>
-        <v>159</v>
+        <v>40</v>
       </c>
       <c r="I33">
         <f>$F$5*31</f>
-        <v>1643</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1418,33 +1472,34 @@
         <v>2015</v>
       </c>
       <c r="B34">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="C34">
         <v>30</v>
       </c>
       <c r="D34" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>42368</v>
+        <v>42338</v>
       </c>
       <c r="F34">
-        <v>1590</v>
+        <f t="shared" si="1"/>
+        <v>1200</v>
       </c>
       <c r="G34">
         <f>WEEKDAY(DATE(A34,B34,C34))</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H34">
         <f>$F$5*G34</f>
-        <v>212</v>
+        <v>80</v>
       </c>
       <c r="I34">
         <f>$F$5*31</f>
-        <v>1643</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1452,37 +1507,39 @@
         <v>2015</v>
       </c>
       <c r="B35">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="C35">
         <v>31</v>
       </c>
       <c r="D35" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E35" s="1">
         <f t="shared" si="0"/>
-        <v>42369</v>
+        <v>42339</v>
       </c>
       <c r="F35">
-        <v>1643</v>
+        <f t="shared" si="1"/>
+        <v>1240</v>
       </c>
       <c r="G35">
         <f>WEEKDAY(DATE(A35,B35,C35))</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H35">
         <f>$F$5*G35</f>
-        <v>265</v>
+        <v>120</v>
       </c>
       <c r="I35">
         <f>$F$5*31</f>
-        <v>1643</v>
+        <v>1240</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>